<commit_message>
feat: agrega notificaciones al manejar boletas
</commit_message>
<xml_diff>
--- a/backend/tests/files_required/data_studiends.xlsx
+++ b/backend/tests/files_required/data_studiends.xlsx
@@ -951,10 +951,10 @@
   <dimension ref="A1:M361"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="C28:M28 D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.12109375" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.55"/>
@@ -2214,8 +2214,8 @@
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
refactor: cambia data de prueba
</commit_message>
<xml_diff>
--- a/backend/tests/files_required/data_studiends.xlsx
+++ b/backend/tests/files_required/data_studiends.xlsx
@@ -951,10 +951,10 @@
   <dimension ref="A1:M361"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="C28:M28 D12"/>
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2:M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.13671875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.15625" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.55"/>

</xml_diff>